<commit_message>
[TEST] in memory tests with fluent nhibernate and sqlite
</commit_message>
<xml_diff>
--- a/Hydra/Hydra.Import.Test/Resources/ExcelHelper.xlsx
+++ b/Hydra/Hydra.Import.Test/Resources/ExcelHelper.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\GRC_Source\Development\Source\GRCKernel\GRCImportUnitTests\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\03 HG\TecX\Hydra\Hydra.Import.Test\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
   </bookViews>
   <sheets>
-    <sheet name="Testzellen" sheetId="1" r:id="rId1"/>
+    <sheet name="Cells" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,20 +24,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Erste Zeile,
-Zweite Zeile</t>
+    <t>First line,
+second line</t>
   </si>
   <si>
-    <t>Eins
-Zwei</t>
+    <t>One
+Two</t>
+  </si>
+  <si>
+    <t>12/18/2014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -67,11 +73,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -352,28 +360,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2">
+        <v>41991</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>